<commit_message>
feat: mock perfectly implemented
</commit_message>
<xml_diff>
--- a/output/common_words/excel/common_words_among_websites_dict.xlsx
+++ b/output/common_words/excel/common_words_among_websites_dict.xlsx
@@ -17,13 +17,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -34,7 +37,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -42,12 +45,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,14 +425,212 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Common Word</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Total Frequency</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Websites</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Cookies</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>83</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>https://www.100-dakar.com (14), https://www.benjaminwahl.at (18), https://www.drehorgelkabarett.at (14), https://www.ottosaxinger.at (3), https://www.peligro.at (14), https://www.schuledesungehorsams.at (2), https://www.skodone.at (18)</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Page</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>35</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>https://www.hungaromedia.at (8), https://www.kuenstlerinnen.at (8), https://www.luckeneder-art.at (8), https://www.platform-socialism.org (3), https://www.regional-express.org (8)</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Linz</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>52</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>https://www.freie-medien.at (10), https://www.freizeitundkommunikation.at (3), https://www.linzfmr.at (18), https://www.steingeschichten.at (21)</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>März</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>49</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>https://www.das-kollektiv.at (8), https://www.feminismus-krawall.at (16), https://www.fiftitu.at (19), https://www.unkraut-comics.at (6)</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Art</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>29</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>https://www.eipcp.net (13), https://www.kairus.org (6), https://www.negentropy-sport.net (2), https://www.radical-openness.org (8)</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Schule</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>294</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>https://www.alteschule-gutau.at (4), https://www.derschueler.at (5), https://www.die-schule.at (285)</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Uhr</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>33</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>https://www.fro.at (21), https://www.rudolfhabringer.at (12)</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Kultur</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>32</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>https://www.frauenkultur.at (17), https://www.igkultur.at (15)</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>15</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>https://www.corpushomini.info (3), https://www.doublehappiness.at (12)</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Magdalena</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>12</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>https://www.magdalenareiter.at (2), https://www.themagdalenaproject.org (10)</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Casino</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>10</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>https://www.frf.at (6), https://www.photosalonhelga.com (4)</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Andreas</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>8</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>https://www.andreaskurz.net (2), https://www.andreaszingerle.com (6)</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
build: architecture is organised
</commit_message>
<xml_diff>
--- a/output/common_words/excel/common_words_among_websites_dict.xlsx
+++ b/output/common_words/excel/common_words_among_websites_dict.xlsx
@@ -17,13 +17,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -34,7 +37,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -42,12 +45,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,14 +425,257 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Common Word</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Total Frequency</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Websites</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Cookies</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>140</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>https://www.100-dakar.com (14), https://www.benjaminwahl.at (18), https://www.dasholzhaus.at (11), https://www.diequote.at (24), https://www.drehorgelkabarett.at (14), https://www.frautomani.at (4), https://www.ingridschiller.at (14), https://www.ottosaxinger.at (3), https://www.peligro.at (14), https://www.reinhardreisenzahn.com (4), https://www.schuledesungehorsams.at (2), https://www.skodone.at (18)</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Linz</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>55</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>https://www.freie-medien.at (10), https://www.freizeitundkommunikation.at (3), https://www.linzfmr.at (18), https://www.pflueckt.at (3), https://www.steingeschichten.at (21)</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Film</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>47</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>https://www.apileofghosts.com (16), https://www.boxafilm.com (8), https://www.corpushomini.info (3), https://www.doublehappiness.at (12), https://www.retrogoldmine.com (8)</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Art</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>45</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>https://www.eipcp.net (13), https://www.faces-l.net (16), https://www.kairus.org (6), https://www.negentropy-sport.net (2), https://www.radical-openness.org (8)</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Page</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>35</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>https://www.hungaromedia.at (8), https://www.kuenstlerinnen.at (8), https://www.luckeneder-art.at (8), https://www.platform-socialism.org (3), https://www.regional-express.org (8)</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>März</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>49</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>https://www.das-kollektiv.at (8), https://www.feminismus-krawall.at (16), https://www.fiftitu.at (19), https://www.unkraut-comics.at (6)</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Schule</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>294</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>https://www.alteschule-gutau.at (4), https://www.derschueler.at (5), https://www.die-schule.at (285)</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Radio</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>175</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>https://www.radio-fri.at (6), https://www.schulradiotag.at (169)</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Mehr</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>64</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>https://www.diebresche.org (23), https://www.programmkinowels.at (41)</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Uhr</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>32</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>https://www.fro.at (20), https://www.rudolfhabringer.at (12)</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Kultur</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>31</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>https://www.frauenkultur.at (17), https://www.igkultur.at (14)</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Magdalena</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>12</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>https://www.magdalenareiter.at (2), https://www.themagdalenaproject.org (10)</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Casino</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>10</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>https://www.frf.at (6), https://www.photosalonhelga.com (4)</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Andreas</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>8</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>https://www.andreaskurz.net (2), https://www.andreaszingerle.com (6)</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Anna</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>8</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>https://www.anna-kraher.de (5), https://www.lllk.at (3)</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
build: file path fixed
</commit_message>
<xml_diff>
--- a/output/common_words/excel/common_words_among_websites_dict.xlsx
+++ b/output/common_words/excel/common_words_among_websites_dict.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -457,221 +457,161 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>140</v>
+        <v>83</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://www.100-dakar.com (14), https://www.benjaminwahl.at (18), https://www.dasholzhaus.at (11), https://www.diequote.at (24), https://www.drehorgelkabarett.at (14), https://www.frautomani.at (4), https://www.ingridschiller.at (14), https://www.ottosaxinger.at (3), https://www.peligro.at (14), https://www.reinhardreisenzahn.com (4), https://www.schuledesungehorsams.at (2), https://www.skodone.at (18)</t>
+          <t>https://www.100-dakar.com (14), https://www.benjaminwahl.at (18), https://www.drehorgelkabarett.at (14), https://www.ottosaxinger.at (3), https://www.peligro.at (14), https://www.schuledesungehorsams.at (2), https://www.skodone.at (18)</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Linz</t>
+          <t>Page</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://www.freie-medien.at (10), https://www.freizeitundkommunikation.at (3), https://www.linzfmr.at (18), https://www.pflueckt.at (3), https://www.steingeschichten.at (21)</t>
+          <t>https://www.hungaromedia.at (8), https://www.kuenstlerinnen.at (8), https://www.luckeneder-art.at (8), https://www.platform-socialism.org (3), https://www.regional-express.org (8)</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Film</t>
+          <t>Linz</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://www.apileofghosts.com (16), https://www.boxafilm.com (8), https://www.corpushomini.info (3), https://www.doublehappiness.at (12), https://www.retrogoldmine.com (8)</t>
+          <t>https://www.freie-medien.at (10), https://www.freizeitundkommunikation.at (3), https://www.linzfmr.at (18), https://www.steingeschichten.at (21)</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Art</t>
+          <t>März</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>https://www.eipcp.net (13), https://www.faces-l.net (16), https://www.kairus.org (6), https://www.negentropy-sport.net (2), https://www.radical-openness.org (8)</t>
+          <t>https://www.das-kollektiv.at (8), https://www.feminismus-krawall.at (16), https://www.fiftitu.at (19), https://www.unkraut-comics.at (6)</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Page</t>
+          <t>Art</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>https://www.hungaromedia.at (8), https://www.kuenstlerinnen.at (8), https://www.luckeneder-art.at (8), https://www.platform-socialism.org (3), https://www.regional-express.org (8)</t>
+          <t>https://www.eipcp.net (13), https://www.kairus.org (6), https://www.negentropy-sport.net (2), https://www.radical-openness.org (8)</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>März</t>
+          <t>Schule</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>49</v>
+        <v>294</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>https://www.das-kollektiv.at (8), https://www.feminismus-krawall.at (16), https://www.fiftitu.at (19), https://www.unkraut-comics.at (6)</t>
+          <t>https://www.alteschule-gutau.at (4), https://www.derschueler.at (5), https://www.die-schule.at (285)</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Schule</t>
+          <t>Uhr</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>294</v>
+        <v>35</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>https://www.alteschule-gutau.at (4), https://www.derschueler.at (5), https://www.die-schule.at (285)</t>
+          <t>https://www.fro.at (23), https://www.rudolfhabringer.at (12)</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Radio</t>
+          <t>Kultur</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>175</v>
+        <v>31</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>https://www.radio-fri.at (6), https://www.schulradiotag.at (169)</t>
+          <t>https://www.frauenkultur.at (17), https://www.igkultur.at (14)</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Mehr</t>
+          <t>Film</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>64</v>
+        <v>15</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>https://www.diebresche.org (23), https://www.programmkinowels.at (41)</t>
+          <t>https://www.corpushomini.info (3), https://www.doublehappiness.at (12)</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Uhr</t>
+          <t>Magdalena</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>https://www.fro.at (20), https://www.rudolfhabringer.at (12)</t>
+          <t>https://www.magdalenareiter.at (2), https://www.themagdalenaproject.org (10)</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Kultur</t>
+          <t>Andreas</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>https://www.frauenkultur.at (17), https://www.igkultur.at (14)</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Magdalena</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>12</v>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>https://www.magdalenareiter.at (2), https://www.themagdalenaproject.org (10)</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Casino</t>
-        </is>
-      </c>
-      <c r="B14" t="n">
-        <v>10</v>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>https://www.frf.at (6), https://www.photosalonhelga.com (4)</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>Andreas</t>
-        </is>
-      </c>
-      <c r="B15" t="n">
-        <v>8</v>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
           <t>https://www.andreaskurz.net (2), https://www.andreaszingerle.com (6)</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>Anna</t>
-        </is>
-      </c>
-      <c r="B16" t="n">
-        <v>8</v>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>https://www.anna-kraher.de (5), https://www.lllk.at (3)</t>
         </is>
       </c>
     </row>

</xml_diff>